<commit_message>
RF/SVM models Louisville using TargetEncoder
</commit_message>
<xml_diff>
--- a/Resources/Results.xlsx
+++ b/Resources/Results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\GitlabContent\project-3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\GitlabContent\project-3\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{407831B2-237E-4966-82D5-3A7FC34E0767}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC89B51-1C9B-45EB-BEF2-EF34E6957F36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="18490" windowHeight="11020" activeTab="1" xr2:uid="{1F03D750-29BA-4508-AE65-8D8AB8484A6A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="352">
   <si>
     <t>Random Forest (Train/Test split)</t>
   </si>
@@ -744,9 +744,6 @@
     <t>n/a</t>
   </si>
   <si>
-    <t>Take out IntakeInternalStatus</t>
-  </si>
-  <si>
     <t>Put back IntakeAsilomarStatus</t>
   </si>
   <si>
@@ -786,34 +783,313 @@
     <t>Put back IntakeInternalStatus - but NEW GROUPS!</t>
   </si>
   <si>
-    <t>IntakeStatus_Normal              0.103230</t>
-  </si>
-  <si>
-    <t>Sex_Male                         0.066257</t>
-  </si>
-  <si>
-    <t>Pet_age_category_Senior          0.052747</t>
-  </si>
-  <si>
-    <t>Pet_age_category_Adult           0.035147</t>
-  </si>
-  <si>
-    <t>BreedCategory_Pure               0.034962</t>
-  </si>
-  <si>
-    <t>Pet_age_category_Young           0.032233</t>
-  </si>
-  <si>
-    <t>PrimaryBreed_PIT BULL TERRIER    0.031817</t>
-  </si>
-  <si>
-    <t>BreedCategory_Two                0.031470</t>
-  </si>
-  <si>
-    <t>IntakeStatus_Other               0.026908</t>
-  </si>
-  <si>
-    <t>IntakeStatus_Sick                0.026796</t>
+    <t>IntakeStatus_Normal                       0.113817</t>
+  </si>
+  <si>
+    <t>Sex_Male                                  0.063265</t>
+  </si>
+  <si>
+    <t>PrimaryBreed_PIT BULL TERRIER             0.052117</t>
+  </si>
+  <si>
+    <t>BreedCategory_Pure                        0.036802</t>
+  </si>
+  <si>
+    <t>BreedCategory_Two                         0.035732</t>
+  </si>
+  <si>
+    <t>IntakeStatus_Sick                         0.033447</t>
+  </si>
+  <si>
+    <t>IntakeStatus_Other                        0.031816</t>
+  </si>
+  <si>
+    <t>PrimaryBreed_AMERICAN PIT BULL TERRIER    0.024750</t>
+  </si>
+  <si>
+    <t>PrimaryColor_BROWN                        0.022309</t>
+  </si>
+  <si>
+    <t>PrimaryColor_BLACK                        0.020418</t>
+  </si>
+  <si>
+    <t>Didn't drop DOB null - kept 20K rows!  Running the model WITHOUT PetAgeCat.  Is sacrificing PetAgeCat for additional 20K InternalStatus makes a difference?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              precision    recall  f1-score   support</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           0       0.78      0.96      0.86     12061</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           1       0.56      0.15      0.24      3863</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    accuracy                           0.77     15924</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   macro avg       0.67      0.56      0.55     15924</t>
+  </si>
+  <si>
+    <t>weighted avg       0.73      0.77      0.71     15924</t>
+  </si>
+  <si>
+    <t>SVM Classification report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           0       0.77      0.98      0.86     12061</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                precision    recall  f1-score   support</t>
+  </si>
+  <si>
+    <t>mse</t>
+  </si>
+  <si>
+    <t>Sex              0.419407</t>
+  </si>
+  <si>
+    <t>IntakeStatus     0.295337</t>
+  </si>
+  <si>
+    <t>BreedCategory    0.249627</t>
+  </si>
+  <si>
+    <t>PrimaryColor     0.035246</t>
+  </si>
+  <si>
+    <t>PrimaryBreed     0.000382</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           1       0.61      0.08      0.14      3863</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    accuracy                           0.76     15924</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   macro avg       0.69      0.53      0.50     15924</t>
+  </si>
+  <si>
+    <t>weighted avg       0.73      0.76      0.69     15924</t>
+  </si>
+  <si>
+    <t>PrimaryBreed             0.655426</t>
+  </si>
+  <si>
+    <t>IntakeStatus_Normal      0.120796</t>
+  </si>
+  <si>
+    <t>IntakeStatus_Sick        0.026762</t>
+  </si>
+  <si>
+    <t>BreedCategory_Two        0.026150</t>
+  </si>
+  <si>
+    <t>IntakeStatus_Other       0.025558</t>
+  </si>
+  <si>
+    <t>Sex_Male                 0.024380</t>
+  </si>
+  <si>
+    <t>BreedCategory_Pure       0.021941</t>
+  </si>
+  <si>
+    <t>PrimaryColor_TRICOLOR    0.008299</t>
+  </si>
+  <si>
+    <t>PrimaryColor_BLACK       0.008237</t>
+  </si>
+  <si>
+    <t>PrimaryColor_BROWN       0.006166</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           0       0.76      1.00      0.86     12025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           1       0.00      0.00      0.00      3899</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   macro avg       0.38      0.50      0.43     15924</t>
+  </si>
+  <si>
+    <t>weighted avg       0.57      0.76      0.65     15924</t>
+  </si>
+  <si>
+    <t>Taking the TOP 25 breeds (account for 80%), all others in "Other"</t>
+  </si>
+  <si>
+    <t>IntakeStatus_Normal                   0.172355</t>
+  </si>
+  <si>
+    <t>TopBreed_PIT BULL TERRIER             0.071767</t>
+  </si>
+  <si>
+    <t>Sex_Male                              0.065411</t>
+  </si>
+  <si>
+    <t>BreedCategory_Two                     0.046587</t>
+  </si>
+  <si>
+    <t>IntakeStatus_Sick                     0.043780</t>
+  </si>
+  <si>
+    <t>BreedCategory_Pure                    0.043313</t>
+  </si>
+  <si>
+    <t>IntakeStatus_Other                    0.041212</t>
+  </si>
+  <si>
+    <t>TopBreed_Other                        0.036402</t>
+  </si>
+  <si>
+    <t>TopBreed_CHIHUAHUA - SMOOTH COATED    0.027596</t>
+  </si>
+  <si>
+    <t>TopBreed_CHOW CHOW                    0.021649</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           0       0.77      0.97      0.86     12025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           1       0.53      0.12      0.19      3899</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   macro avg       0.65      0.54      0.53     15924</t>
+  </si>
+  <si>
+    <t>weighted avg       0.71      0.76      0.70     15924</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TESTING using COUNT/FREQUENCY encoding on Primary Breed</t>
+  </si>
+  <si>
+    <t>TESTING using TARGETENCODER()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TESTING using LeaveOneOutEncoder()</t>
+  </si>
+  <si>
+    <t>DEALING WITH HIGH CARDINALITY (WITH PRIMARY BREED COLUMN/COLOR)</t>
+  </si>
+  <si>
+    <t>PrimaryBreed     0.562639</t>
+  </si>
+  <si>
+    <t>IntakeStatus     0.187577</t>
+  </si>
+  <si>
+    <t>PrimaryColor     0.185061</t>
+  </si>
+  <si>
+    <t>BreedCategory    0.044305</t>
+  </si>
+  <si>
+    <t>Sex              0.020418</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           0       0.77      0.98      0.86     12025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           1       0.59      0.09      0.16      3899</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   macro avg       0.68      0.54      0.51     15924</t>
+  </si>
+  <si>
+    <t>weighted avg       0.72      0.76      0.69     15924</t>
+  </si>
+  <si>
+    <t>FINAL LOGIC!</t>
+  </si>
+  <si>
+    <t>PetAgeCategory</t>
+  </si>
+  <si>
+    <t>PetAgeCategory - DID NOT USE / DROPPED</t>
+  </si>
+  <si>
+    <t>Took out IntakeInternalStatus</t>
+  </si>
+  <si>
+    <t>IntakeStatus_Normal              0.099756</t>
+  </si>
+  <si>
+    <t>Sex_Male                         0.070188</t>
+  </si>
+  <si>
+    <t>PetAgeCategory_Senior            0.055192</t>
+  </si>
+  <si>
+    <t>BreedCategory_Pure               0.037071</t>
+  </si>
+  <si>
+    <t>PrimaryBreed_PIT BULL TERRIER    0.032865</t>
+  </si>
+  <si>
+    <t>PetAgeCategory_Adult             0.032434</t>
+  </si>
+  <si>
+    <t>PetAgeCategory_Young             0.031989</t>
+  </si>
+  <si>
+    <t>BreedCategory_Two                0.027843</t>
+  </si>
+  <si>
+    <t>IntakeStatus_Other               0.026667</t>
+  </si>
+  <si>
+    <t>IntakeStatus_Sick                0.026658</t>
+  </si>
+  <si>
+    <t>?????</t>
+  </si>
+  <si>
+    <t>Agree witk Kelly. PetAgeMonth will be useful   in the future even though now, the accuracy is lower.   Go to FINAL logic!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           0       0.76      0.86      0.81      7087</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           1       0.58      0.41      0.48      3297</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    accuracy                           0.72     10384</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   macro avg       0.67      0.63      0.64     10384</t>
+  </si>
+  <si>
+    <t>weighted avg       0.70      0.72      0.70     10384</t>
+  </si>
+  <si>
+    <t>TARGETENCODER()</t>
+  </si>
+  <si>
+    <t>PrimaryBreed      0.461202</t>
+  </si>
+  <si>
+    <t>PrimaryColor      0.211202</t>
+  </si>
+  <si>
+    <t>IntakeStatus      0.152061</t>
+  </si>
+  <si>
+    <t>PetAgeCategory    0.109951</t>
+  </si>
+  <si>
+    <t>BreedCategory     0.041580</t>
+  </si>
+  <si>
+    <t>Sex               0.024004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           0       0.75      0.89      0.81      7087</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           1       0.60      0.35      0.45      3297</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   macro avg       0.67      0.62      0.63     10384</t>
   </si>
 </sst>
 </file>
@@ -884,7 +1160,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -909,8 +1185,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -933,11 +1227,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -994,12 +1325,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1007,15 +1332,106 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1032,6 +1448,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1876,13 +2296,13 @@
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
-      <c r="M11" s="26" t="s">
+      <c r="M11" s="31" t="s">
         <v>138</v>
       </c>
-      <c r="N11" s="27"/>
-      <c r="O11" s="27"/>
-      <c r="P11" s="27"/>
-      <c r="Q11" s="28"/>
+      <c r="N11" s="32"/>
+      <c r="O11" s="32"/>
+      <c r="P11" s="32"/>
+      <c r="Q11" s="33"/>
       <c r="R11" s="6" t="s">
         <v>175</v>
       </c>
@@ -3058,10 +3478,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8A8C2BF-9908-41B9-981E-FAB4544CDCE3}">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:P44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3069,26 +3489,40 @@
     <col min="1" max="1" width="11.26953125" customWidth="1"/>
     <col min="2" max="2" width="14.08984375" customWidth="1"/>
     <col min="3" max="3" width="16.54296875" customWidth="1"/>
-    <col min="4" max="4" width="32.08984375" customWidth="1"/>
-    <col min="5" max="6" width="40.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="14.90625" customWidth="1"/>
+    <col min="4" max="4" width="32.08984375" style="38" customWidth="1"/>
+    <col min="5" max="6" width="40.54296875" style="38" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.54296875" style="38" customWidth="1"/>
+    <col min="8" max="8" width="40.54296875" style="38" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.54296875" style="38" customWidth="1"/>
+    <col min="10" max="12" width="40.54296875" style="38" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="14.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="21"/>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-    </row>
-    <row r="2" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="59" t="s">
+        <v>321</v>
+      </c>
+      <c r="G1" s="60"/>
+      <c r="H1" s="41" t="s">
+        <v>336</v>
+      </c>
+      <c r="I1" s="48" t="s">
+        <v>311</v>
+      </c>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+    </row>
+    <row r="2" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="24" t="s">
         <v>14</v>
       </c>
@@ -3096,45 +3530,69 @@
       <c r="C2" s="24" t="s">
         <v>214</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="41" t="s">
         <v>214</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="41" t="s">
         <v>214</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="43" t="s">
         <v>214</v>
       </c>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="24"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="G2" s="43" t="s">
+        <v>214</v>
+      </c>
+      <c r="H2" s="41" t="s">
+        <v>214</v>
+      </c>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="24"/>
+    </row>
+    <row r="3" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
       <c r="C3" s="24" t="s">
         <v>233</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="41" t="s">
         <v>233</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="41" t="s">
         <v>233</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="43" t="s">
         <v>233</v>
       </c>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="G3" s="42" t="s">
+        <v>342</v>
+      </c>
+      <c r="H3" s="41" t="s">
+        <v>233</v>
+      </c>
+      <c r="I3" s="42" t="s">
+        <v>293</v>
+      </c>
+      <c r="J3" s="42" t="s">
+        <v>308</v>
+      </c>
+      <c r="K3" s="42" t="s">
+        <v>309</v>
+      </c>
+      <c r="L3" s="51" t="s">
+        <v>310</v>
+      </c>
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="24"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="24"/>
       <c r="B4" s="24" t="s">
         <v>7</v>
@@ -3142,23 +3600,39 @@
       <c r="C4" s="24" t="s">
         <v>215</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="41" t="s">
         <v>215</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="41" t="s">
         <v>215</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="43" t="s">
         <v>215</v>
       </c>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="G4" s="43" t="s">
+        <v>215</v>
+      </c>
+      <c r="H4" s="41" t="s">
+        <v>215</v>
+      </c>
+      <c r="I4" s="41" t="s">
+        <v>215</v>
+      </c>
+      <c r="J4" s="41" t="s">
+        <v>215</v>
+      </c>
+      <c r="K4" s="41" t="s">
+        <v>215</v>
+      </c>
+      <c r="L4" s="50" t="s">
+        <v>215</v>
+      </c>
+      <c r="M4" s="22"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="24"/>
+      <c r="P4" s="24"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="24"/>
       <c r="B5" s="24" t="s">
         <v>8</v>
@@ -3166,23 +3640,39 @@
       <c r="C5" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="24" t="s">
+      <c r="F5" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24"/>
-      <c r="L5" s="24"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="G5" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="K5" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="L5" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="M5" s="22"/>
+      <c r="N5" s="22"/>
+      <c r="O5" s="24"/>
+      <c r="P5" s="24"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="24"/>
       <c r="B6" s="24" t="s">
         <v>9</v>
@@ -3190,23 +3680,39 @@
       <c r="C6" s="24" t="s">
         <v>216</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="41" t="s">
         <v>216</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="41" t="s">
         <v>216</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="F6" s="43" t="s">
         <v>216</v>
       </c>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="G6" s="43" t="s">
+        <v>216</v>
+      </c>
+      <c r="H6" s="41" t="s">
+        <v>216</v>
+      </c>
+      <c r="I6" s="41" t="s">
+        <v>216</v>
+      </c>
+      <c r="J6" s="41" t="s">
+        <v>216</v>
+      </c>
+      <c r="K6" s="41" t="s">
+        <v>216</v>
+      </c>
+      <c r="L6" s="50" t="s">
+        <v>216</v>
+      </c>
+      <c r="M6" s="22"/>
+      <c r="N6" s="22"/>
+      <c r="O6" s="24"/>
+      <c r="P6" s="24"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="24"/>
       <c r="B7" s="24" t="s">
         <v>234</v>
@@ -3214,344 +3720,905 @@
       <c r="C7" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="D7" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="E7" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="F7" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24"/>
-      <c r="L7" s="24"/>
-    </row>
-    <row r="8" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="D7" s="41" t="s">
+        <v>322</v>
+      </c>
+      <c r="E7" s="41" t="s">
+        <v>322</v>
+      </c>
+      <c r="F7" s="43" t="s">
+        <v>322</v>
+      </c>
+      <c r="G7" s="43" t="s">
+        <v>322</v>
+      </c>
+      <c r="H7" s="41" t="s">
+        <v>322</v>
+      </c>
+      <c r="I7" s="42" t="s">
+        <v>323</v>
+      </c>
+      <c r="J7" s="42" t="s">
+        <v>323</v>
+      </c>
+      <c r="K7" s="42" t="s">
+        <v>323</v>
+      </c>
+      <c r="L7" s="42" t="s">
+        <v>323</v>
+      </c>
+      <c r="M7" s="22"/>
+      <c r="N7" s="22"/>
+      <c r="O7" s="24"/>
+      <c r="P7" s="24"/>
+    </row>
+    <row r="8" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="24"/>
       <c r="B8" s="24"/>
       <c r="C8" s="24" t="s">
         <v>217</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="41" t="s">
         <v>218</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="41" t="s">
         <v>218</v>
       </c>
-      <c r="F8" s="24" t="s">
+      <c r="F8" s="43" t="s">
         <v>218</v>
       </c>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="24"/>
-    </row>
-    <row r="9" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="G8" s="43" t="s">
+        <v>218</v>
+      </c>
+      <c r="H8" s="41" t="s">
+        <v>218</v>
+      </c>
+      <c r="I8" s="41" t="s">
+        <v>218</v>
+      </c>
+      <c r="J8" s="41" t="s">
+        <v>218</v>
+      </c>
+      <c r="K8" s="41" t="s">
+        <v>218</v>
+      </c>
+      <c r="L8" s="50" t="s">
+        <v>218</v>
+      </c>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22"/>
+      <c r="O8" s="24"/>
+      <c r="P8" s="24"/>
+    </row>
+    <row r="9" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="24"/>
       <c r="B9" s="24"/>
       <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24" t="s">
-        <v>236</v>
-      </c>
-      <c r="F9" s="24" t="s">
-        <v>249</v>
-      </c>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="24"/>
-      <c r="J9" s="24"/>
-      <c r="K9" s="24"/>
-      <c r="L9" s="24"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="D9" s="41"/>
+      <c r="E9" s="41" t="s">
+        <v>324</v>
+      </c>
+      <c r="F9" s="43" t="s">
+        <v>248</v>
+      </c>
+      <c r="G9" s="43" t="s">
+        <v>248</v>
+      </c>
+      <c r="H9" s="41" t="s">
+        <v>248</v>
+      </c>
+      <c r="I9" s="41" t="s">
+        <v>248</v>
+      </c>
+      <c r="J9" s="41" t="s">
+        <v>248</v>
+      </c>
+      <c r="K9" s="41" t="s">
+        <v>248</v>
+      </c>
+      <c r="L9" s="50" t="s">
+        <v>248</v>
+      </c>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="24"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="24"/>
       <c r="B10" s="24"/>
       <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24" t="s">
-        <v>237</v>
-      </c>
-      <c r="F10" s="24" t="s">
-        <v>248</v>
-      </c>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="24"/>
-    </row>
-    <row r="11" spans="1:12" s="32" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A11" s="29" t="s">
+      <c r="D10" s="41"/>
+      <c r="E10" s="41" t="s">
+        <v>236</v>
+      </c>
+      <c r="F10" s="43" t="s">
+        <v>247</v>
+      </c>
+      <c r="G10" s="43" t="s">
+        <v>247</v>
+      </c>
+      <c r="H10" s="41" t="s">
+        <v>247</v>
+      </c>
+      <c r="I10" s="41" t="s">
+        <v>247</v>
+      </c>
+      <c r="J10" s="41" t="s">
+        <v>247</v>
+      </c>
+      <c r="K10" s="41" t="s">
+        <v>247</v>
+      </c>
+      <c r="L10" s="50" t="s">
+        <v>247</v>
+      </c>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="24"/>
+    </row>
+    <row r="11" spans="1:16" ht="58" x14ac:dyDescent="0.35">
+      <c r="A11" s="26"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="42" t="s">
+        <v>259</v>
+      </c>
+      <c r="I11" s="43" t="s">
+        <v>259</v>
+      </c>
+      <c r="J11" s="43" t="s">
+        <v>259</v>
+      </c>
+      <c r="K11" s="43" t="s">
+        <v>259</v>
+      </c>
+      <c r="L11" s="52" t="s">
+        <v>259</v>
+      </c>
+      <c r="M11" s="22"/>
+      <c r="N11" s="22"/>
+      <c r="O11" s="26"/>
+      <c r="P11" s="26"/>
+    </row>
+    <row r="12" spans="1:16" s="29" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A12" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B12" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="30">
+      <c r="C12" s="28">
         <v>0.71</v>
       </c>
-      <c r="D11" s="31">
+      <c r="D12" s="36">
         <v>0.70889999999999997</v>
       </c>
-      <c r="E11" s="31">
+      <c r="E12" s="36">
         <v>0.69350000000000001</v>
       </c>
-      <c r="F11" s="31">
-        <v>0.70509999999999995</v>
-      </c>
-      <c r="G11" s="31"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="30"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="30"/>
-      <c r="L11" s="30"/>
-    </row>
-    <row r="12" spans="1:12" s="32" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="29" t="s">
+      <c r="F12" s="36">
+        <v>0.70220000000000005</v>
+      </c>
+      <c r="G12" s="36">
+        <v>0.69889999999999997</v>
+      </c>
+      <c r="H12" s="36">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="I12" s="36">
+        <v>0.75439999999999996</v>
+      </c>
+      <c r="J12" s="36">
+        <v>0.74980000000000002</v>
+      </c>
+      <c r="K12" s="36">
+        <v>0.753</v>
+      </c>
+      <c r="L12" s="53">
         <v>1</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="M12" s="55"/>
+      <c r="N12" s="55"/>
+      <c r="O12" s="28"/>
+      <c r="P12" s="28"/>
+    </row>
+    <row r="13" spans="1:16" s="29" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="30"/>
-      <c r="D12" s="31">
+      <c r="C13" s="28"/>
+      <c r="D13" s="36">
         <v>0.7006</v>
       </c>
-      <c r="E12" s="31">
+      <c r="E13" s="36">
         <v>0.68640000000000001</v>
       </c>
-      <c r="F12" s="31">
-        <v>0.69910000000000005</v>
-      </c>
-      <c r="G12" s="31"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="30"/>
-      <c r="L12" s="30"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
-        <v>143</v>
-      </c>
+      <c r="F13" s="36">
+        <v>0.7</v>
+      </c>
+      <c r="G13" s="36">
+        <v>0.69669999999999999</v>
+      </c>
+      <c r="H13" s="36">
+        <v>0.75349999999999995</v>
+      </c>
+      <c r="I13" s="36">
+        <v>0.75380000000000003</v>
+      </c>
+      <c r="J13" s="36">
+        <v>0.74760000000000004</v>
+      </c>
+      <c r="K13" s="36">
+        <v>0.75019999999999998</v>
+      </c>
+      <c r="L13" s="53">
+        <v>1</v>
+      </c>
+      <c r="M13" s="55"/>
+      <c r="N13" s="55"/>
+      <c r="O13" s="28"/>
+      <c r="P13" s="28"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="11"/>
-      <c r="D14" s="3">
-        <v>0.72</v>
-      </c>
-      <c r="E14" s="3">
-        <v>0.69799999999999995</v>
-      </c>
-      <c r="F14" s="3">
-        <v>0.71799999999999997</v>
-      </c>
-      <c r="G14" s="3"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
-    </row>
-    <row r="15" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="37"/>
+      <c r="L14" s="54"/>
+      <c r="M14" s="22"/>
+      <c r="N14" s="22"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>176</v>
+        <v>143</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="11"/>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="37">
+        <v>0.72</v>
+      </c>
+      <c r="E15" s="37">
+        <v>0.69799999999999995</v>
+      </c>
+      <c r="F15" s="36">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="G15" s="36">
+        <v>0.72</v>
+      </c>
+      <c r="H15" s="37">
+        <v>0.76500000000000001</v>
+      </c>
+      <c r="I15" s="37">
+        <v>0.75870000000000004</v>
+      </c>
+      <c r="J15" s="37">
+        <v>0.75509999999999999</v>
+      </c>
+      <c r="K15" s="37">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="L15" s="54">
+        <v>0.76400000000000001</v>
+      </c>
+      <c r="M15" s="22"/>
+      <c r="N15" s="22"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11"/>
+    </row>
+    <row r="16" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="37" t="s">
         <v>235</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E16" s="37" t="s">
         <v>235</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="G15" s="3"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="33" t="s">
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="37"/>
+      <c r="L16" s="54"/>
+      <c r="M16" s="22"/>
+      <c r="N16" s="22"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A18" s="30" t="s">
         <v>229</v>
       </c>
-      <c r="D17">
+      <c r="D18" s="38">
         <v>274</v>
       </c>
-      <c r="E17">
+      <c r="E18" s="38">
         <v>253</v>
       </c>
-      <c r="F17">
+      <c r="F18" s="47">
         <v>255</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="33" t="s">
+      <c r="G18" s="47">
+        <v>6</v>
+      </c>
+      <c r="H18" s="38">
+        <v>261</v>
+      </c>
+      <c r="I18" s="38">
+        <v>77</v>
+      </c>
+      <c r="J18" s="38">
+        <v>53</v>
+      </c>
+      <c r="K18" s="38">
+        <v>5</v>
+      </c>
+      <c r="L18" s="38">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="F19" s="47"/>
+      <c r="G19" s="47"/>
+    </row>
+    <row r="20" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="30" t="s">
         <v>230</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D20" s="44" t="s">
         <v>219</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E20" s="44" t="s">
+        <v>237</v>
+      </c>
+      <c r="F20" s="56" t="s">
+        <v>325</v>
+      </c>
+      <c r="G20" s="39" t="s">
+        <v>343</v>
+      </c>
+      <c r="H20" s="44" t="s">
+        <v>249</v>
+      </c>
+      <c r="I20" s="39" t="s">
+        <v>294</v>
+      </c>
+      <c r="J20" s="44" t="s">
+        <v>279</v>
+      </c>
+      <c r="K20" s="39" t="s">
+        <v>312</v>
+      </c>
+      <c r="L20" s="44" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="D21" s="44" t="s">
+        <v>220</v>
+      </c>
+      <c r="E21" s="44" t="s">
         <v>238</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="F21" s="56" t="s">
+        <v>326</v>
+      </c>
+      <c r="G21" s="39" t="s">
+        <v>344</v>
+      </c>
+      <c r="H21" s="44" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D20" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="E20" s="5" t="s">
+      <c r="I21" s="39" t="s">
+        <v>295</v>
+      </c>
+      <c r="J21" s="44" t="s">
+        <v>280</v>
+      </c>
+      <c r="K21" s="39" t="s">
+        <v>313</v>
+      </c>
+      <c r="L21" s="44" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="D22" s="44" t="s">
+        <v>221</v>
+      </c>
+      <c r="E22" s="44" t="s">
         <v>239</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="F22" s="56" t="s">
+        <v>327</v>
+      </c>
+      <c r="G22" s="39" t="s">
+        <v>345</v>
+      </c>
+      <c r="H22" s="44" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D21" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="E21" s="5" t="s">
+      <c r="I22" s="39" t="s">
+        <v>296</v>
+      </c>
+      <c r="J22" s="44" t="s">
+        <v>281</v>
+      </c>
+      <c r="K22" s="39" t="s">
+        <v>314</v>
+      </c>
+      <c r="L22" s="44" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="D23" s="44" t="s">
+        <v>222</v>
+      </c>
+      <c r="E23" s="44" t="s">
         <v>240</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="F23" s="56" t="s">
+        <v>328</v>
+      </c>
+      <c r="G23" s="39" t="s">
+        <v>346</v>
+      </c>
+      <c r="H23" s="44" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D22" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="E22" s="5" t="s">
+      <c r="I23" s="39" t="s">
+        <v>297</v>
+      </c>
+      <c r="J23" s="44" t="s">
+        <v>282</v>
+      </c>
+      <c r="K23" s="39" t="s">
+        <v>315</v>
+      </c>
+      <c r="L23" s="44" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="D24" s="44" t="s">
+        <v>223</v>
+      </c>
+      <c r="E24" s="44" t="s">
         <v>241</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="F24" s="56" t="s">
+        <v>329</v>
+      </c>
+      <c r="G24" s="39" t="s">
+        <v>347</v>
+      </c>
+      <c r="H24" s="44" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D23" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="E23" s="5" t="s">
+      <c r="I24" s="39" t="s">
+        <v>298</v>
+      </c>
+      <c r="J24" s="44" t="s">
+        <v>283</v>
+      </c>
+      <c r="K24" s="39" t="s">
+        <v>316</v>
+      </c>
+      <c r="L24" s="44" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="D25" s="44" t="s">
+        <v>224</v>
+      </c>
+      <c r="E25" s="44" t="s">
         <v>242</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F25" s="56" t="s">
+        <v>330</v>
+      </c>
+      <c r="G25" s="39" t="s">
+        <v>348</v>
+      </c>
+      <c r="H25" s="44" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D24" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="E24" s="5" t="s">
+      <c r="I25" s="39" t="s">
+        <v>299</v>
+      </c>
+      <c r="J25" s="44" t="s">
+        <v>284</v>
+      </c>
+      <c r="K25" s="44"/>
+      <c r="L25" s="44"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="D26" s="44" t="s">
+        <v>225</v>
+      </c>
+      <c r="E26" s="44" t="s">
         <v>243</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="F26" s="56" t="s">
+        <v>331</v>
+      </c>
+      <c r="G26" s="56"/>
+      <c r="H26" s="44" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D25" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="E25" s="5" t="s">
+      <c r="I26" s="39" t="s">
+        <v>300</v>
+      </c>
+      <c r="J26" s="44" t="s">
+        <v>285</v>
+      </c>
+      <c r="K26" s="44"/>
+      <c r="L26" s="44"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="D27" s="44" t="s">
+        <v>226</v>
+      </c>
+      <c r="E27" s="44" t="s">
         <v>244</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="F27" s="56" t="s">
+        <v>332</v>
+      </c>
+      <c r="G27" s="56"/>
+      <c r="H27" s="44" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D26" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="E26" s="5" t="s">
+      <c r="I27" s="39" t="s">
+        <v>301</v>
+      </c>
+      <c r="J27" s="44" t="s">
+        <v>286</v>
+      </c>
+      <c r="K27" s="44"/>
+      <c r="L27" s="44"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="D28" s="44" t="s">
+        <v>227</v>
+      </c>
+      <c r="E28" s="44" t="s">
         <v>245</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="F28" s="56" t="s">
+        <v>333</v>
+      </c>
+      <c r="G28" s="56"/>
+      <c r="H28" s="44" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D27" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="E27" s="5" t="s">
+      <c r="I28" s="39" t="s">
+        <v>302</v>
+      </c>
+      <c r="J28" s="44" t="s">
+        <v>287</v>
+      </c>
+      <c r="K28" s="44"/>
+      <c r="L28" s="44"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="D29" s="44" t="s">
+        <v>228</v>
+      </c>
+      <c r="E29" s="44" t="s">
         <v>246</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="F29" s="56" t="s">
+        <v>334</v>
+      </c>
+      <c r="G29" s="56"/>
+      <c r="H29" s="44" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D28" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+      <c r="I29" s="39" t="s">
+        <v>303</v>
+      </c>
+      <c r="J29" s="44" t="s">
+        <v>288</v>
+      </c>
+      <c r="K29" s="44"/>
+      <c r="L29" s="44"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>231</v>
       </c>
-      <c r="D30" s="34">
+      <c r="D31" s="45">
         <v>1243812</v>
       </c>
-      <c r="E30" s="34">
+      <c r="E31" s="45">
         <v>1009324</v>
       </c>
-      <c r="F30" s="34">
-        <v>1233646</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+      <c r="F31" s="61">
+        <v>1196702</v>
+      </c>
+      <c r="G31" s="61">
+        <v>968594</v>
+      </c>
+      <c r="H31" s="45">
+        <v>987366</v>
+      </c>
+      <c r="I31" s="40">
+        <v>1145876</v>
+      </c>
+      <c r="J31" s="45">
+        <v>1580118</v>
+      </c>
+      <c r="K31" s="40">
+        <v>1594580</v>
+      </c>
+      <c r="L31" s="40">
+        <v>6356</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>232</v>
       </c>
-      <c r="D31" s="5">
+      <c r="D32" s="44">
         <v>123</v>
       </c>
-      <c r="E31" s="5">
+      <c r="E32" s="44">
         <v>127.5</v>
       </c>
-      <c r="F31" s="5">
-        <v>121</v>
-      </c>
+      <c r="F32" s="62">
+        <v>122</v>
+      </c>
+      <c r="G32" s="62">
+        <v>29</v>
+      </c>
+      <c r="H32" s="44">
+        <v>149</v>
+      </c>
+      <c r="I32" s="44">
+        <v>51</v>
+      </c>
+      <c r="J32" s="44">
+        <v>47</v>
+      </c>
+      <c r="K32" s="44">
+        <v>28</v>
+      </c>
+      <c r="L32" s="44">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>269</v>
+      </c>
+      <c r="F33" s="63">
+        <v>49.39</v>
+      </c>
+      <c r="G33" s="63">
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="H33" s="38">
+        <v>0.46579999999999999</v>
+      </c>
+      <c r="I33" s="47">
+        <v>0.2455</v>
+      </c>
+      <c r="J33" s="47" t="s">
+        <v>335</v>
+      </c>
+      <c r="K33" s="38">
+        <v>0.24690000000000001</v>
+      </c>
+      <c r="L33" s="46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="F34" s="47"/>
+      <c r="G34" s="47"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>266</v>
+      </c>
+      <c r="F35" s="57" t="s">
+        <v>260</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="H35" s="44" t="s">
+        <v>268</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="K35" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="L35" s="44" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="F36" s="58"/>
+      <c r="G36" s="34"/>
+      <c r="I36" s="34"/>
+      <c r="J36" s="34"/>
+      <c r="K36" s="34"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="F37" s="57" t="s">
+        <v>337</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="H37" s="44" t="s">
+        <v>261</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="K37" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="L37" s="44" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="F38" s="57" t="s">
+        <v>338</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="H38" s="44" t="s">
+        <v>262</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="K38" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="L38" s="44" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="F39" s="58"/>
+      <c r="G39" s="34"/>
+      <c r="I39" s="34"/>
+      <c r="J39" s="34"/>
+      <c r="K39" s="34"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="F40" s="57" t="s">
+        <v>339</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="H40" s="44" t="s">
+        <v>263</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="J40" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="K40" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="L40" s="44" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="F41" s="57" t="s">
+        <v>340</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="H41" s="44" t="s">
+        <v>264</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="J41" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="K41" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="L41" s="44" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="F42" s="57" t="s">
+        <v>341</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="H42" s="44" t="s">
+        <v>265</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="J42" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="K42" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="L42" s="44" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="F43" s="47"/>
+      <c r="G43" s="47"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="F44" s="47"/>
+      <c r="G44" s="47"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Cleaning up RF model code
</commit_message>
<xml_diff>
--- a/Resources/Results.xlsx
+++ b/Resources/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\GitlabContent\project-3\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC89B51-1C9B-45EB-BEF2-EF34E6957F36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AFEFEAF-A898-416E-9562-2DBE90BD8AE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="18490" windowHeight="11020" activeTab="1" xr2:uid="{1F03D750-29BA-4508-AE65-8D8AB8484A6A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="353">
   <si>
     <t>Random Forest (Train/Test split)</t>
   </si>
@@ -1090,6 +1090,9 @@
   </si>
   <si>
     <t xml:space="preserve">   macro avg       0.67      0.62      0.63     10384</t>
+  </si>
+  <si>
+    <t>OneHotEncoder()</t>
   </si>
 </sst>
 </file>
@@ -1336,15 +1339,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1386,12 +1380,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -1418,20 +1406,35 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1448,10 +1451,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2296,13 +2295,13 @@
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
-      <c r="M11" s="31" t="s">
+      <c r="M11" s="57" t="s">
         <v>138</v>
       </c>
-      <c r="N11" s="32"/>
-      <c r="O11" s="32"/>
-      <c r="P11" s="32"/>
-      <c r="Q11" s="33"/>
+      <c r="N11" s="58"/>
+      <c r="O11" s="58"/>
+      <c r="P11" s="58"/>
+      <c r="Q11" s="59"/>
       <c r="R11" s="6" t="s">
         <v>175</v>
       </c>
@@ -3480,8 +3479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8A8C2BF-9908-41B9-981E-FAB4544CDCE3}">
   <dimension ref="A1:P44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3489,12 +3488,12 @@
     <col min="1" max="1" width="11.26953125" customWidth="1"/>
     <col min="2" max="2" width="14.08984375" customWidth="1"/>
     <col min="3" max="3" width="16.54296875" customWidth="1"/>
-    <col min="4" max="4" width="32.08984375" style="38" customWidth="1"/>
-    <col min="5" max="6" width="40.54296875" style="38" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="40.54296875" style="38" customWidth="1"/>
-    <col min="8" max="8" width="40.54296875" style="38" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="40.54296875" style="38" customWidth="1"/>
-    <col min="10" max="12" width="40.54296875" style="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.08984375" style="35" customWidth="1"/>
+    <col min="5" max="6" width="40.54296875" style="35" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.54296875" style="35" customWidth="1"/>
+    <col min="8" max="8" width="40.54296875" style="35" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.54296875" style="35" customWidth="1"/>
+    <col min="10" max="12" width="40.54296875" style="35" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="14.90625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3502,21 +3501,21 @@
       <c r="A1" s="21"/>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="59" t="s">
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="62" t="s">
         <v>321</v>
       </c>
-      <c r="G1" s="60"/>
-      <c r="H1" s="41" t="s">
+      <c r="G1" s="63"/>
+      <c r="H1" s="38" t="s">
         <v>336</v>
       </c>
-      <c r="I1" s="48" t="s">
+      <c r="I1" s="60" t="s">
         <v>311</v>
       </c>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
       <c r="M1" s="22"/>
       <c r="N1" s="22"/>
       <c r="O1" s="22"/>
@@ -3530,25 +3529,25 @@
       <c r="C2" s="24" t="s">
         <v>214</v>
       </c>
-      <c r="D2" s="41" t="s">
+      <c r="D2" s="38" t="s">
         <v>214</v>
       </c>
-      <c r="E2" s="41" t="s">
+      <c r="E2" s="38" t="s">
         <v>214</v>
       </c>
-      <c r="F2" s="43" t="s">
+      <c r="F2" s="40" t="s">
         <v>214</v>
       </c>
-      <c r="G2" s="43" t="s">
+      <c r="G2" s="40" t="s">
         <v>214</v>
       </c>
-      <c r="H2" s="41" t="s">
+      <c r="H2" s="38" t="s">
         <v>214</v>
       </c>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="50"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="45"/>
       <c r="M2" s="22"/>
       <c r="N2" s="22"/>
       <c r="O2" s="10"/>
@@ -3560,31 +3559,31 @@
       <c r="C3" s="24" t="s">
         <v>233</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="38" t="s">
         <v>233</v>
       </c>
-      <c r="E3" s="41" t="s">
+      <c r="E3" s="38" t="s">
         <v>233</v>
       </c>
-      <c r="F3" s="43" t="s">
+      <c r="F3" s="40" t="s">
+        <v>352</v>
+      </c>
+      <c r="G3" s="39" t="s">
+        <v>342</v>
+      </c>
+      <c r="H3" s="38" t="s">
         <v>233</v>
       </c>
-      <c r="G3" s="42" t="s">
-        <v>342</v>
-      </c>
-      <c r="H3" s="41" t="s">
-        <v>233</v>
-      </c>
-      <c r="I3" s="42" t="s">
+      <c r="I3" s="39" t="s">
         <v>293</v>
       </c>
-      <c r="J3" s="42" t="s">
+      <c r="J3" s="39" t="s">
         <v>308</v>
       </c>
-      <c r="K3" s="42" t="s">
+      <c r="K3" s="39" t="s">
         <v>309</v>
       </c>
-      <c r="L3" s="51" t="s">
+      <c r="L3" s="46" t="s">
         <v>310</v>
       </c>
       <c r="M3" s="22"/>
@@ -3600,31 +3599,31 @@
       <c r="C4" s="24" t="s">
         <v>215</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="38" t="s">
         <v>215</v>
       </c>
-      <c r="E4" s="41" t="s">
+      <c r="E4" s="38" t="s">
         <v>215</v>
       </c>
-      <c r="F4" s="43" t="s">
+      <c r="F4" s="40" t="s">
         <v>215</v>
       </c>
-      <c r="G4" s="43" t="s">
+      <c r="G4" s="40" t="s">
         <v>215</v>
       </c>
-      <c r="H4" s="41" t="s">
+      <c r="H4" s="38" t="s">
         <v>215</v>
       </c>
-      <c r="I4" s="41" t="s">
+      <c r="I4" s="38" t="s">
         <v>215</v>
       </c>
-      <c r="J4" s="41" t="s">
+      <c r="J4" s="38" t="s">
         <v>215</v>
       </c>
-      <c r="K4" s="41" t="s">
+      <c r="K4" s="38" t="s">
         <v>215</v>
       </c>
-      <c r="L4" s="50" t="s">
+      <c r="L4" s="45" t="s">
         <v>215</v>
       </c>
       <c r="M4" s="22"/>
@@ -3640,31 +3639,31 @@
       <c r="C5" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="41" t="s">
+      <c r="D5" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="43" t="s">
+      <c r="F5" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="43" t="s">
+      <c r="G5" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="41" t="s">
+      <c r="H5" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="41" t="s">
+      <c r="I5" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="41" t="s">
+      <c r="J5" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="41" t="s">
+      <c r="K5" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="L5" s="50" t="s">
+      <c r="L5" s="45" t="s">
         <v>6</v>
       </c>
       <c r="M5" s="22"/>
@@ -3680,31 +3679,31 @@
       <c r="C6" s="24" t="s">
         <v>216</v>
       </c>
-      <c r="D6" s="41" t="s">
+      <c r="D6" s="38" t="s">
         <v>216</v>
       </c>
-      <c r="E6" s="41" t="s">
+      <c r="E6" s="38" t="s">
         <v>216</v>
       </c>
-      <c r="F6" s="43" t="s">
+      <c r="F6" s="40" t="s">
         <v>216</v>
       </c>
-      <c r="G6" s="43" t="s">
+      <c r="G6" s="40" t="s">
         <v>216</v>
       </c>
-      <c r="H6" s="41" t="s">
+      <c r="H6" s="38" t="s">
         <v>216</v>
       </c>
-      <c r="I6" s="41" t="s">
+      <c r="I6" s="38" t="s">
         <v>216</v>
       </c>
-      <c r="J6" s="41" t="s">
+      <c r="J6" s="38" t="s">
         <v>216</v>
       </c>
-      <c r="K6" s="41" t="s">
+      <c r="K6" s="38" t="s">
         <v>216</v>
       </c>
-      <c r="L6" s="50" t="s">
+      <c r="L6" s="45" t="s">
         <v>216</v>
       </c>
       <c r="M6" s="22"/>
@@ -3720,31 +3719,31 @@
       <c r="C7" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="D7" s="41" t="s">
+      <c r="D7" s="38" t="s">
         <v>322</v>
       </c>
-      <c r="E7" s="41" t="s">
+      <c r="E7" s="38" t="s">
         <v>322</v>
       </c>
-      <c r="F7" s="43" t="s">
+      <c r="F7" s="40" t="s">
         <v>322</v>
       </c>
-      <c r="G7" s="43" t="s">
+      <c r="G7" s="40" t="s">
         <v>322</v>
       </c>
-      <c r="H7" s="41" t="s">
+      <c r="H7" s="38" t="s">
         <v>322</v>
       </c>
-      <c r="I7" s="42" t="s">
+      <c r="I7" s="39" t="s">
         <v>323</v>
       </c>
-      <c r="J7" s="42" t="s">
+      <c r="J7" s="39" t="s">
         <v>323</v>
       </c>
-      <c r="K7" s="42" t="s">
+      <c r="K7" s="39" t="s">
         <v>323</v>
       </c>
-      <c r="L7" s="42" t="s">
+      <c r="L7" s="39" t="s">
         <v>323</v>
       </c>
       <c r="M7" s="22"/>
@@ -3758,31 +3757,31 @@
       <c r="C8" s="24" t="s">
         <v>217</v>
       </c>
-      <c r="D8" s="41" t="s">
+      <c r="D8" s="38" t="s">
         <v>218</v>
       </c>
-      <c r="E8" s="41" t="s">
+      <c r="E8" s="38" t="s">
         <v>218</v>
       </c>
-      <c r="F8" s="43" t="s">
+      <c r="F8" s="40" t="s">
         <v>218</v>
       </c>
-      <c r="G8" s="43" t="s">
+      <c r="G8" s="40" t="s">
         <v>218</v>
       </c>
-      <c r="H8" s="41" t="s">
+      <c r="H8" s="38" t="s">
         <v>218</v>
       </c>
-      <c r="I8" s="41" t="s">
+      <c r="I8" s="38" t="s">
         <v>218</v>
       </c>
-      <c r="J8" s="41" t="s">
+      <c r="J8" s="38" t="s">
         <v>218</v>
       </c>
-      <c r="K8" s="41" t="s">
+      <c r="K8" s="38" t="s">
         <v>218</v>
       </c>
-      <c r="L8" s="50" t="s">
+      <c r="L8" s="45" t="s">
         <v>218</v>
       </c>
       <c r="M8" s="22"/>
@@ -3794,29 +3793,29 @@
       <c r="A9" s="24"/>
       <c r="B9" s="24"/>
       <c r="C9" s="24"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41" t="s">
+      <c r="D9" s="38"/>
+      <c r="E9" s="38" t="s">
         <v>324</v>
       </c>
-      <c r="F9" s="43" t="s">
+      <c r="F9" s="40" t="s">
         <v>248</v>
       </c>
-      <c r="G9" s="43" t="s">
+      <c r="G9" s="40" t="s">
         <v>248</v>
       </c>
-      <c r="H9" s="41" t="s">
+      <c r="H9" s="38" t="s">
         <v>248</v>
       </c>
-      <c r="I9" s="41" t="s">
+      <c r="I9" s="38" t="s">
         <v>248</v>
       </c>
-      <c r="J9" s="41" t="s">
+      <c r="J9" s="38" t="s">
         <v>248</v>
       </c>
-      <c r="K9" s="41" t="s">
+      <c r="K9" s="38" t="s">
         <v>248</v>
       </c>
-      <c r="L9" s="50" t="s">
+      <c r="L9" s="45" t="s">
         <v>248</v>
       </c>
       <c r="M9" s="22"/>
@@ -3828,29 +3827,29 @@
       <c r="A10" s="24"/>
       <c r="B10" s="24"/>
       <c r="C10" s="24"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41" t="s">
+      <c r="D10" s="38"/>
+      <c r="E10" s="38" t="s">
         <v>236</v>
       </c>
-      <c r="F10" s="43" t="s">
+      <c r="F10" s="40" t="s">
         <v>247</v>
       </c>
-      <c r="G10" s="43" t="s">
+      <c r="G10" s="40" t="s">
         <v>247</v>
       </c>
-      <c r="H10" s="41" t="s">
+      <c r="H10" s="38" t="s">
         <v>247</v>
       </c>
-      <c r="I10" s="41" t="s">
+      <c r="I10" s="38" t="s">
         <v>247</v>
       </c>
-      <c r="J10" s="41" t="s">
+      <c r="J10" s="38" t="s">
         <v>247</v>
       </c>
-      <c r="K10" s="41" t="s">
+      <c r="K10" s="38" t="s">
         <v>247</v>
       </c>
-      <c r="L10" s="50" t="s">
+      <c r="L10" s="45" t="s">
         <v>247</v>
       </c>
       <c r="M10" s="22"/>
@@ -3862,23 +3861,23 @@
       <c r="A11" s="26"/>
       <c r="B11" s="26"/>
       <c r="C11" s="26"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="42" t="s">
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="39" t="s">
         <v>259</v>
       </c>
-      <c r="I11" s="43" t="s">
+      <c r="I11" s="40" t="s">
         <v>259</v>
       </c>
-      <c r="J11" s="43" t="s">
+      <c r="J11" s="40" t="s">
         <v>259</v>
       </c>
-      <c r="K11" s="43" t="s">
+      <c r="K11" s="40" t="s">
         <v>259</v>
       </c>
-      <c r="L11" s="52" t="s">
+      <c r="L11" s="47" t="s">
         <v>259</v>
       </c>
       <c r="M11" s="22"/>
@@ -3896,35 +3895,35 @@
       <c r="C12" s="28">
         <v>0.71</v>
       </c>
-      <c r="D12" s="36">
+      <c r="D12" s="33">
         <v>0.70889999999999997</v>
       </c>
-      <c r="E12" s="36">
+      <c r="E12" s="33">
         <v>0.69350000000000001</v>
       </c>
-      <c r="F12" s="36">
-        <v>0.70220000000000005</v>
-      </c>
-      <c r="G12" s="36">
+      <c r="F12" s="33">
+        <v>0.70469999999999999</v>
+      </c>
+      <c r="G12" s="33">
         <v>0.69889999999999997</v>
       </c>
-      <c r="H12" s="36">
+      <c r="H12" s="33">
         <v>0.75600000000000001</v>
       </c>
-      <c r="I12" s="36">
+      <c r="I12" s="33">
         <v>0.75439999999999996</v>
       </c>
-      <c r="J12" s="36">
+      <c r="J12" s="33">
         <v>0.74980000000000002</v>
       </c>
-      <c r="K12" s="36">
+      <c r="K12" s="33">
         <v>0.753</v>
       </c>
-      <c r="L12" s="53">
+      <c r="L12" s="48">
         <v>1</v>
       </c>
-      <c r="M12" s="55"/>
-      <c r="N12" s="55"/>
+      <c r="M12" s="50"/>
+      <c r="N12" s="50"/>
       <c r="O12" s="28"/>
       <c r="P12" s="28"/>
     </row>
@@ -3936,35 +3935,35 @@
         <v>12</v>
       </c>
       <c r="C13" s="28"/>
-      <c r="D13" s="36">
+      <c r="D13" s="33">
         <v>0.7006</v>
       </c>
-      <c r="E13" s="36">
+      <c r="E13" s="33">
         <v>0.68640000000000001</v>
       </c>
-      <c r="F13" s="36">
-        <v>0.7</v>
-      </c>
-      <c r="G13" s="36">
+      <c r="F13" s="33">
+        <v>0.69799999999999995</v>
+      </c>
+      <c r="G13" s="33">
         <v>0.69669999999999999</v>
       </c>
-      <c r="H13" s="36">
+      <c r="H13" s="33">
         <v>0.75349999999999995</v>
       </c>
-      <c r="I13" s="36">
+      <c r="I13" s="33">
         <v>0.75380000000000003</v>
       </c>
-      <c r="J13" s="36">
+      <c r="J13" s="33">
         <v>0.74760000000000004</v>
       </c>
-      <c r="K13" s="36">
+      <c r="K13" s="33">
         <v>0.75019999999999998</v>
       </c>
-      <c r="L13" s="53">
+      <c r="L13" s="48">
         <v>1</v>
       </c>
-      <c r="M13" s="55"/>
-      <c r="N13" s="55"/>
+      <c r="M13" s="50"/>
+      <c r="N13" s="50"/>
       <c r="O13" s="28"/>
       <c r="P13" s="28"/>
     </row>
@@ -3972,15 +3971,15 @@
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="11"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="37"/>
-      <c r="K14" s="37"/>
-      <c r="L14" s="54"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="49"/>
       <c r="M14" s="22"/>
       <c r="N14" s="22"/>
       <c r="O14" s="11"/>
@@ -3992,31 +3991,31 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="11"/>
-      <c r="D15" s="37">
+      <c r="D15" s="34">
         <v>0.72</v>
       </c>
-      <c r="E15" s="37">
+      <c r="E15" s="34">
         <v>0.69799999999999995</v>
       </c>
-      <c r="F15" s="36">
-        <v>0.71699999999999997</v>
-      </c>
-      <c r="G15" s="36">
+      <c r="F15" s="33">
+        <v>0.71389999999999998</v>
+      </c>
+      <c r="G15" s="33">
         <v>0.72</v>
       </c>
-      <c r="H15" s="37">
+      <c r="H15" s="34">
         <v>0.76500000000000001</v>
       </c>
-      <c r="I15" s="37">
+      <c r="I15" s="34">
         <v>0.75870000000000004</v>
       </c>
-      <c r="J15" s="37">
+      <c r="J15" s="34">
         <v>0.75509999999999999</v>
       </c>
-      <c r="K15" s="37">
+      <c r="K15" s="34">
         <v>0.76200000000000001</v>
       </c>
-      <c r="L15" s="54">
+      <c r="L15" s="49">
         <v>0.76400000000000001</v>
       </c>
       <c r="M15" s="22"/>
@@ -4030,362 +4029,364 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="11"/>
-      <c r="D16" s="37" t="s">
+      <c r="D16" s="34" t="s">
         <v>235</v>
       </c>
-      <c r="E16" s="37" t="s">
+      <c r="E16" s="34" t="s">
         <v>235</v>
       </c>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="37"/>
-      <c r="K16" s="37"/>
-      <c r="L16" s="54"/>
+      <c r="F16" s="33">
+        <v>0.70240000000000002</v>
+      </c>
+      <c r="G16" s="33"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="49"/>
       <c r="M16" s="22"/>
       <c r="N16" s="22"/>
       <c r="O16" s="11"/>
       <c r="P16" s="11"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="30" t="s">
         <v>229</v>
       </c>
-      <c r="D18" s="38">
+      <c r="D18" s="35">
         <v>274</v>
       </c>
-      <c r="E18" s="38">
+      <c r="E18" s="35">
         <v>253</v>
       </c>
-      <c r="F18" s="47">
+      <c r="F18" s="44">
         <v>255</v>
       </c>
-      <c r="G18" s="47">
+      <c r="G18" s="44">
         <v>6</v>
       </c>
-      <c r="H18" s="38">
+      <c r="H18" s="35">
         <v>261</v>
       </c>
-      <c r="I18" s="38">
+      <c r="I18" s="35">
         <v>77</v>
       </c>
-      <c r="J18" s="38">
+      <c r="J18" s="35">
         <v>53</v>
       </c>
-      <c r="K18" s="38">
+      <c r="K18" s="35">
         <v>5</v>
       </c>
-      <c r="L18" s="38">
+      <c r="L18" s="35">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="F19" s="47"/>
-      <c r="G19" s="47"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="44"/>
     </row>
     <row r="20" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="30" t="s">
         <v>230</v>
       </c>
-      <c r="D20" s="44" t="s">
+      <c r="D20" s="41" t="s">
         <v>219</v>
       </c>
-      <c r="E20" s="44" t="s">
+      <c r="E20" s="41" t="s">
         <v>237</v>
       </c>
-      <c r="F20" s="56" t="s">
+      <c r="F20" s="51" t="s">
         <v>325</v>
       </c>
-      <c r="G20" s="39" t="s">
+      <c r="G20" s="36" t="s">
         <v>343</v>
       </c>
-      <c r="H20" s="44" t="s">
+      <c r="H20" s="41" t="s">
         <v>249</v>
       </c>
-      <c r="I20" s="39" t="s">
+      <c r="I20" s="36" t="s">
         <v>294</v>
       </c>
-      <c r="J20" s="44" t="s">
+      <c r="J20" s="41" t="s">
         <v>279</v>
       </c>
-      <c r="K20" s="39" t="s">
+      <c r="K20" s="36" t="s">
         <v>312</v>
       </c>
-      <c r="L20" s="44" t="s">
+      <c r="L20" s="41" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D21" s="44" t="s">
+      <c r="D21" s="41" t="s">
         <v>220</v>
       </c>
-      <c r="E21" s="44" t="s">
+      <c r="E21" s="41" t="s">
         <v>238</v>
       </c>
-      <c r="F21" s="56" t="s">
+      <c r="F21" s="51" t="s">
         <v>326</v>
       </c>
-      <c r="G21" s="39" t="s">
+      <c r="G21" s="36" t="s">
         <v>344</v>
       </c>
-      <c r="H21" s="44" t="s">
+      <c r="H21" s="41" t="s">
         <v>250</v>
       </c>
-      <c r="I21" s="39" t="s">
+      <c r="I21" s="36" t="s">
         <v>295</v>
       </c>
-      <c r="J21" s="44" t="s">
+      <c r="J21" s="41" t="s">
         <v>280</v>
       </c>
-      <c r="K21" s="39" t="s">
+      <c r="K21" s="36" t="s">
         <v>313</v>
       </c>
-      <c r="L21" s="44" t="s">
+      <c r="L21" s="41" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D22" s="44" t="s">
+      <c r="D22" s="41" t="s">
         <v>221</v>
       </c>
-      <c r="E22" s="44" t="s">
+      <c r="E22" s="41" t="s">
         <v>239</v>
       </c>
-      <c r="F22" s="56" t="s">
+      <c r="F22" s="51" t="s">
         <v>327</v>
       </c>
-      <c r="G22" s="39" t="s">
+      <c r="G22" s="36" t="s">
         <v>345</v>
       </c>
-      <c r="H22" s="44" t="s">
+      <c r="H22" s="41" t="s">
         <v>251</v>
       </c>
-      <c r="I22" s="39" t="s">
+      <c r="I22" s="36" t="s">
         <v>296</v>
       </c>
-      <c r="J22" s="44" t="s">
+      <c r="J22" s="41" t="s">
         <v>281</v>
       </c>
-      <c r="K22" s="39" t="s">
+      <c r="K22" s="36" t="s">
         <v>314</v>
       </c>
-      <c r="L22" s="44" t="s">
+      <c r="L22" s="41" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D23" s="44" t="s">
+      <c r="D23" s="41" t="s">
         <v>222</v>
       </c>
-      <c r="E23" s="44" t="s">
+      <c r="E23" s="41" t="s">
         <v>240</v>
       </c>
-      <c r="F23" s="56" t="s">
+      <c r="F23" s="51" t="s">
         <v>328</v>
       </c>
-      <c r="G23" s="39" t="s">
+      <c r="G23" s="36" t="s">
         <v>346</v>
       </c>
-      <c r="H23" s="44" t="s">
+      <c r="H23" s="41" t="s">
         <v>252</v>
       </c>
-      <c r="I23" s="39" t="s">
+      <c r="I23" s="36" t="s">
         <v>297</v>
       </c>
-      <c r="J23" s="44" t="s">
+      <c r="J23" s="41" t="s">
         <v>282</v>
       </c>
-      <c r="K23" s="39" t="s">
+      <c r="K23" s="36" t="s">
         <v>315</v>
       </c>
-      <c r="L23" s="44" t="s">
+      <c r="L23" s="41" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D24" s="44" t="s">
+      <c r="D24" s="41" t="s">
         <v>223</v>
       </c>
-      <c r="E24" s="44" t="s">
+      <c r="E24" s="41" t="s">
         <v>241</v>
       </c>
-      <c r="F24" s="56" t="s">
+      <c r="F24" s="51" t="s">
         <v>329</v>
       </c>
-      <c r="G24" s="39" t="s">
+      <c r="G24" s="36" t="s">
         <v>347</v>
       </c>
-      <c r="H24" s="44" t="s">
+      <c r="H24" s="41" t="s">
         <v>253</v>
       </c>
-      <c r="I24" s="39" t="s">
+      <c r="I24" s="36" t="s">
         <v>298</v>
       </c>
-      <c r="J24" s="44" t="s">
+      <c r="J24" s="41" t="s">
         <v>283</v>
       </c>
-      <c r="K24" s="39" t="s">
+      <c r="K24" s="36" t="s">
         <v>316</v>
       </c>
-      <c r="L24" s="44" t="s">
+      <c r="L24" s="41" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D25" s="44" t="s">
+      <c r="D25" s="41" t="s">
         <v>224</v>
       </c>
-      <c r="E25" s="44" t="s">
+      <c r="E25" s="41" t="s">
         <v>242</v>
       </c>
-      <c r="F25" s="56" t="s">
+      <c r="F25" s="51" t="s">
         <v>330</v>
       </c>
-      <c r="G25" s="39" t="s">
+      <c r="G25" s="36" t="s">
         <v>348</v>
       </c>
-      <c r="H25" s="44" t="s">
+      <c r="H25" s="41" t="s">
         <v>254</v>
       </c>
-      <c r="I25" s="39" t="s">
+      <c r="I25" s="36" t="s">
         <v>299</v>
       </c>
-      <c r="J25" s="44" t="s">
+      <c r="J25" s="41" t="s">
         <v>284</v>
       </c>
-      <c r="K25" s="44"/>
-      <c r="L25" s="44"/>
+      <c r="K25" s="41"/>
+      <c r="L25" s="41"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D26" s="44" t="s">
+      <c r="D26" s="41" t="s">
         <v>225</v>
       </c>
-      <c r="E26" s="44" t="s">
+      <c r="E26" s="41" t="s">
         <v>243</v>
       </c>
-      <c r="F26" s="56" t="s">
+      <c r="F26" s="51" t="s">
         <v>331</v>
       </c>
-      <c r="G26" s="56"/>
-      <c r="H26" s="44" t="s">
+      <c r="G26" s="51"/>
+      <c r="H26" s="41" t="s">
         <v>255</v>
       </c>
-      <c r="I26" s="39" t="s">
+      <c r="I26" s="36" t="s">
         <v>300</v>
       </c>
-      <c r="J26" s="44" t="s">
+      <c r="J26" s="41" t="s">
         <v>285</v>
       </c>
-      <c r="K26" s="44"/>
-      <c r="L26" s="44"/>
+      <c r="K26" s="41"/>
+      <c r="L26" s="41"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D27" s="44" t="s">
+      <c r="D27" s="41" t="s">
         <v>226</v>
       </c>
-      <c r="E27" s="44" t="s">
+      <c r="E27" s="41" t="s">
         <v>244</v>
       </c>
-      <c r="F27" s="56" t="s">
+      <c r="F27" s="51" t="s">
         <v>332</v>
       </c>
-      <c r="G27" s="56"/>
-      <c r="H27" s="44" t="s">
+      <c r="G27" s="51"/>
+      <c r="H27" s="41" t="s">
         <v>256</v>
       </c>
-      <c r="I27" s="39" t="s">
+      <c r="I27" s="36" t="s">
         <v>301</v>
       </c>
-      <c r="J27" s="44" t="s">
+      <c r="J27" s="41" t="s">
         <v>286</v>
       </c>
-      <c r="K27" s="44"/>
-      <c r="L27" s="44"/>
+      <c r="K27" s="41"/>
+      <c r="L27" s="41"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D28" s="44" t="s">
+      <c r="D28" s="41" t="s">
         <v>227</v>
       </c>
-      <c r="E28" s="44" t="s">
+      <c r="E28" s="41" t="s">
         <v>245</v>
       </c>
-      <c r="F28" s="56" t="s">
+      <c r="F28" s="51" t="s">
         <v>333</v>
       </c>
-      <c r="G28" s="56"/>
-      <c r="H28" s="44" t="s">
+      <c r="G28" s="51"/>
+      <c r="H28" s="41" t="s">
         <v>257</v>
       </c>
-      <c r="I28" s="39" t="s">
+      <c r="I28" s="36" t="s">
         <v>302</v>
       </c>
-      <c r="J28" s="44" t="s">
+      <c r="J28" s="41" t="s">
         <v>287</v>
       </c>
-      <c r="K28" s="44"/>
-      <c r="L28" s="44"/>
+      <c r="K28" s="41"/>
+      <c r="L28" s="41"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D29" s="44" t="s">
+      <c r="D29" s="41" t="s">
         <v>228</v>
       </c>
-      <c r="E29" s="44" t="s">
+      <c r="E29" s="41" t="s">
         <v>246</v>
       </c>
-      <c r="F29" s="56" t="s">
+      <c r="F29" s="51" t="s">
         <v>334</v>
       </c>
-      <c r="G29" s="56"/>
-      <c r="H29" s="44" t="s">
+      <c r="G29" s="51"/>
+      <c r="H29" s="41" t="s">
         <v>258</v>
       </c>
-      <c r="I29" s="39" t="s">
+      <c r="I29" s="36" t="s">
         <v>303</v>
       </c>
-      <c r="J29" s="44" t="s">
+      <c r="J29" s="41" t="s">
         <v>288</v>
       </c>
-      <c r="K29" s="44"/>
-      <c r="L29" s="44"/>
+      <c r="K29" s="41"/>
+      <c r="L29" s="41"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="F30" s="47"/>
-      <c r="G30" s="47"/>
+      <c r="F30" s="44"/>
+      <c r="G30" s="44"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>231</v>
       </c>
-      <c r="D31" s="45">
+      <c r="D31" s="42">
         <v>1243812</v>
       </c>
-      <c r="E31" s="45">
+      <c r="E31" s="42">
         <v>1009324</v>
       </c>
-      <c r="F31" s="61">
-        <v>1196702</v>
-      </c>
-      <c r="G31" s="61">
+      <c r="F31" s="54">
+        <v>756962</v>
+      </c>
+      <c r="G31" s="54">
         <v>968594</v>
       </c>
-      <c r="H31" s="45">
+      <c r="H31" s="42">
         <v>987366</v>
       </c>
-      <c r="I31" s="40">
+      <c r="I31" s="37">
         <v>1145876</v>
       </c>
-      <c r="J31" s="45">
+      <c r="J31" s="42">
         <v>1580118</v>
       </c>
-      <c r="K31" s="40">
+      <c r="K31" s="37">
         <v>1594580</v>
       </c>
-      <c r="L31" s="40">
+      <c r="L31" s="37">
         <v>6356</v>
       </c>
     </row>
@@ -4393,31 +4394,31 @@
       <c r="A32" t="s">
         <v>232</v>
       </c>
-      <c r="D32" s="44">
+      <c r="D32" s="41">
         <v>123</v>
       </c>
-      <c r="E32" s="44">
+      <c r="E32" s="41">
         <v>127.5</v>
       </c>
-      <c r="F32" s="62">
-        <v>122</v>
-      </c>
-      <c r="G32" s="62">
+      <c r="F32" s="55">
+        <v>43</v>
+      </c>
+      <c r="G32" s="55">
         <v>29</v>
       </c>
-      <c r="H32" s="44">
+      <c r="H32" s="41">
         <v>149</v>
       </c>
-      <c r="I32" s="44">
+      <c r="I32" s="41">
         <v>51</v>
       </c>
-      <c r="J32" s="44">
+      <c r="J32" s="41">
         <v>47</v>
       </c>
-      <c r="K32" s="44">
+      <c r="K32" s="41">
         <v>28</v>
       </c>
-      <c r="L32" s="44">
+      <c r="L32" s="41">
         <v>11</v>
       </c>
     </row>
@@ -4425,43 +4426,43 @@
       <c r="A33" t="s">
         <v>269</v>
       </c>
-      <c r="F33" s="63">
-        <v>49.39</v>
-      </c>
-      <c r="G33" s="63">
+      <c r="F33" s="56">
+        <v>0.29520000000000002</v>
+      </c>
+      <c r="G33" s="56">
         <v>0.30099999999999999</v>
       </c>
-      <c r="H33" s="38">
+      <c r="H33" s="35">
         <v>0.46579999999999999</v>
       </c>
-      <c r="I33" s="47">
+      <c r="I33" s="44">
         <v>0.2455</v>
       </c>
-      <c r="J33" s="47" t="s">
+      <c r="J33" s="44" t="s">
         <v>335</v>
       </c>
-      <c r="K33" s="38">
+      <c r="K33" s="35">
         <v>0.24690000000000001</v>
       </c>
-      <c r="L33" s="46">
+      <c r="L33" s="43">
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="F34" s="47"/>
-      <c r="G34" s="47"/>
+      <c r="F34" s="44"/>
+      <c r="G34" s="44"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>266</v>
       </c>
-      <c r="F35" s="57" t="s">
+      <c r="F35" s="52" t="s">
         <v>260</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="H35" s="44" t="s">
+      <c r="H35" s="41" t="s">
         <v>268</v>
       </c>
       <c r="I35" s="5" t="s">
@@ -4473,25 +4474,25 @@
       <c r="K35" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="L35" s="44" t="s">
+      <c r="L35" s="41" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="F36" s="58"/>
-      <c r="G36" s="34"/>
-      <c r="I36" s="34"/>
-      <c r="J36" s="34"/>
-      <c r="K36" s="34"/>
+      <c r="F36" s="53"/>
+      <c r="G36" s="31"/>
+      <c r="I36" s="31"/>
+      <c r="J36" s="31"/>
+      <c r="K36" s="31"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="F37" s="57" t="s">
+      <c r="F37" s="52" t="s">
         <v>337</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="H37" s="44" t="s">
+      <c r="H37" s="41" t="s">
         <v>261</v>
       </c>
       <c r="I37" s="5" t="s">
@@ -4503,18 +4504,18 @@
       <c r="K37" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="L37" s="44" t="s">
+      <c r="L37" s="41" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="F38" s="57" t="s">
+      <c r="F38" s="52" t="s">
         <v>338</v>
       </c>
       <c r="G38" s="5" t="s">
         <v>350</v>
       </c>
-      <c r="H38" s="44" t="s">
+      <c r="H38" s="41" t="s">
         <v>262</v>
       </c>
       <c r="I38" s="5" t="s">
@@ -4526,25 +4527,25 @@
       <c r="K38" s="5" t="s">
         <v>318</v>
       </c>
-      <c r="L38" s="44" t="s">
+      <c r="L38" s="41" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="F39" s="58"/>
-      <c r="G39" s="34"/>
-      <c r="I39" s="34"/>
-      <c r="J39" s="34"/>
-      <c r="K39" s="34"/>
+      <c r="F39" s="53"/>
+      <c r="G39" s="31"/>
+      <c r="I39" s="31"/>
+      <c r="J39" s="31"/>
+      <c r="K39" s="31"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="F40" s="57" t="s">
+      <c r="F40" s="52" t="s">
         <v>339</v>
       </c>
       <c r="G40" s="5" t="s">
         <v>339</v>
       </c>
-      <c r="H40" s="44" t="s">
+      <c r="H40" s="41" t="s">
         <v>263</v>
       </c>
       <c r="I40" s="5" t="s">
@@ -4556,18 +4557,18 @@
       <c r="K40" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="L40" s="44" t="s">
+      <c r="L40" s="41" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="F41" s="57" t="s">
+      <c r="F41" s="52" t="s">
         <v>340</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>351</v>
       </c>
-      <c r="H41" s="44" t="s">
+      <c r="H41" s="41" t="s">
         <v>264</v>
       </c>
       <c r="I41" s="5" t="s">
@@ -4579,18 +4580,18 @@
       <c r="K41" s="5" t="s">
         <v>319</v>
       </c>
-      <c r="L41" s="44" t="s">
+      <c r="L41" s="41" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="F42" s="57" t="s">
+      <c r="F42" s="52" t="s">
         <v>341</v>
       </c>
       <c r="G42" s="5" t="s">
         <v>341</v>
       </c>
-      <c r="H42" s="44" t="s">
+      <c r="H42" s="41" t="s">
         <v>265</v>
       </c>
       <c r="I42" s="5" t="s">
@@ -4602,17 +4603,17 @@
       <c r="K42" s="5" t="s">
         <v>320</v>
       </c>
-      <c r="L42" s="44" t="s">
+      <c r="L42" s="41" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="F43" s="47"/>
-      <c r="G43" s="47"/>
+      <c r="F43" s="44"/>
+      <c r="G43" s="44"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="F44" s="47"/>
-      <c r="G44" s="47"/>
+      <c r="F44" s="44"/>
+      <c r="G44" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Changes to final notebooks
</commit_message>
<xml_diff>
--- a/Resources/Results.xlsx
+++ b/Resources/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\GitlabContent\project-3\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E9493C-47F8-44C2-BAD1-ABECD24EC11A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD842E4-B4B1-411A-B897-10380AD5A60F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="18490" windowHeight="11020" activeTab="1" xr2:uid="{1F03D750-29BA-4508-AE65-8D8AB8484A6A}"/>
   </bookViews>
@@ -1752,8 +1752,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAAF7CC1-A9BF-42AE-91D3-8A7A36BD33AD}">
   <dimension ref="A1:AD70"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="6840" ySplit="2170" topLeftCell="H3" activePane="bottomRight"/>
+      <selection pane="topRight" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3480,10 +3483,10 @@
   <dimension ref="A1:P44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3190" ySplit="1200" topLeftCell="I1" activePane="bottomRight"/>
+      <pane xSplit="3190" ySplit="1200" topLeftCell="C1" activePane="bottomRight"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>